<commit_message>
pratibedan change for sarbajanik dhara as per milan sir written, paropakar demolition actual quantity measure, kalimasta mandir estimate given to upabhokta
</commit_message>
<xml_diff>
--- a/ofc/estimates/kalimasta mandir/v.xlsx
+++ b/ofc/estimates/kalimasta mandir/v.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Estimate" sheetId="1" r:id="rId1"/>
@@ -33,14 +33,15 @@
     <definedName name="description_781">[5]Abstract!$B$299</definedName>
     <definedName name="description_783">[1]Abstract!$B$301</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">WCR!$A$1:$K$29</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Estimate!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -247,16 +248,19 @@
   </si>
   <si>
     <t>-slab top bars along y-axis</t>
+  </si>
+  <si>
+    <t>-secondary beam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -422,21 +426,21 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -452,7 +456,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -477,7 +481,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -485,7 +489,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -514,7 +518,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -528,7 +532,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -544,7 +548,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -560,7 +564,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -570,26 +574,23 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -601,6 +602,51 @@
     <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -609,48 +655,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1292,135 +1296,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I64" sqref="I64"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A55" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="64" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-    </row>
-    <row r="2" spans="1:11" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="65" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+    </row>
+    <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="66" t="s">
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="66" t="s">
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-    </row>
-    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="67" t="s">
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="62" t="s">
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="63" t="s">
+      <c r="H6" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="69" t="s">
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="70" t="s">
+      <c r="H7" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="70"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1455,11 +1458,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A9" s="59">
         <v>1</v>
       </c>
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="62" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="29"/>
@@ -1472,7 +1475,7 @@
       <c r="J9" s="29"/>
       <c r="K9" s="29"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="59"/>
       <c r="B10" s="10" t="s">
         <v>57</v>
@@ -1498,7 +1501,7 @@
       <c r="J10" s="29"/>
       <c r="K10" s="29"/>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="10" t="s">
         <v>58</v>
@@ -1524,7 +1527,7 @@
       <c r="J11" s="21"/>
       <c r="K11" s="13"/>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="10"/>
       <c r="C12" s="43">
@@ -1548,7 +1551,7 @@
       <c r="J12" s="21"/>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
         <v>60</v>
@@ -1574,7 +1577,7 @@
       <c r="J13" s="21"/>
       <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
         <v>56</v>
@@ -1592,7 +1595,7 @@
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="20">
-        <f t="shared" ref="G14:G15" si="0">PRODUCT(C14:F14)</f>
+        <f t="shared" ref="G14:G16" si="0">PRODUCT(C14:F14)</f>
         <v>55.489657603032647</v>
       </c>
       <c r="H14" s="21"/>
@@ -1600,7 +1603,7 @@
       <c r="J14" s="21"/>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="10" t="s">
         <v>61</v>
@@ -1625,127 +1628,125 @@
       <c r="J15" s="21"/>
       <c r="K15" s="13"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14">
-        <f>0*SUM(G10:G15)</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="I16" s="14">
-        <v>915.42</v>
-      </c>
-      <c r="J16" s="16">
-        <f>G16*I16</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="13"/>
-    </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="59"/>
+      <c r="B16" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="65">
+        <v>2</v>
+      </c>
+      <c r="D16" s="64">
+        <f>12.25/3.281</f>
+        <v>3.7336177994513866</v>
+      </c>
+      <c r="E16" s="19">
+        <f>0.23*2</f>
+        <v>0.46</v>
+      </c>
+      <c r="F16" s="64"/>
+      <c r="G16" s="30">
+        <f t="shared" si="0"/>
+        <v>3.434928375495276</v>
+      </c>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="12"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="14"/>
+      <c r="G17" s="14">
+        <f>SUM(G10:G16)</f>
+        <v>88.774680461917129</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="14">
+        <v>915.42</v>
+      </c>
       <c r="J17" s="16">
-        <f>0.13*G16*46827.87/100</f>
-        <v>0</v>
+        <f>G17*I17</f>
+        <v>81266.117988448168</v>
       </c>
       <c r="K17" s="13"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="59"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-    </row>
-    <row r="19" spans="1:11" s="17" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="16">
+        <f>0.13*G17*46827.87/100</f>
+        <v>5404.2679547508551</v>
+      </c>
+      <c r="K18" s="13"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="59"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+    </row>
+    <row r="20" spans="1:11" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="25">
         <v>2</v>
       </c>
-      <c r="B19" s="85" t="s">
+      <c r="B20" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C20" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D20" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E20" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F20" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="28"/>
-    </row>
-    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25"/>
-      <c r="B20" s="10" t="s">
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="28"/>
+    </row>
+    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="22">
-        <f>6*(TRUNC((F10/2)/0.15,0)+TRUNC((F10/2)/0.1,0)-4)</f>
-        <v>96</v>
-      </c>
-      <c r="D20" s="23">
-        <f>(7/12/3.281)*4+0.05*2</f>
-        <v>0.81116529513359747</v>
-      </c>
-      <c r="E20" s="23">
-        <f>8*8/162</f>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F20" s="23">
-        <f>PRODUCT(C20:E20)</f>
-        <v>30.764194896918656</v>
-      </c>
-      <c r="G20" s="23">
-        <f>F20/1000</f>
-        <v>3.0764194896918656E-2</v>
-      </c>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="18"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="59"/>
-      <c r="B21" s="29"/>
       <c r="C21" s="22">
         <f>6*(TRUNC((F10/2)/0.15,0)+TRUNC((F10/2)/0.1,0)-4)</f>
         <v>96</v>
       </c>
-      <c r="D21" s="30">
-        <f>0.15*4+0.05*2</f>
-        <v>0.7</v>
+      <c r="D21" s="23">
+        <f>(7/12/3.281)*4+0.05*2</f>
+        <v>0.81116529513359747</v>
       </c>
       <c r="E21" s="23">
         <f>8*8/162</f>
@@ -1753,228 +1754,226 @@
       </c>
       <c r="F21" s="23">
         <f>PRODUCT(C21:E21)</f>
-        <v>26.548148148148144</v>
+        <v>30.764194896918656</v>
       </c>
       <c r="G21" s="23">
         <f>F21/1000</f>
+        <v>3.0764194896918656E-2</v>
+      </c>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="18"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="59"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="22">
+        <f>6*(TRUNC((F10/2)/0.15,0)+TRUNC((F10/2)/0.1,0)-4)</f>
+        <v>96</v>
+      </c>
+      <c r="D22" s="30">
+        <f>0.15*4+0.05*2</f>
+        <v>0.7</v>
+      </c>
+      <c r="E22" s="23">
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F22" s="23">
+        <f>PRODUCT(C22:E22)</f>
+        <v>26.548148148148144</v>
+      </c>
+      <c r="G22" s="23">
+        <f>F22/1000</f>
         <v>2.6548148148148144E-2</v>
-      </c>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="59"/>
-      <c r="B22" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="22">
-        <f>2*5</f>
-        <v>10</v>
-      </c>
-      <c r="D22" s="30">
-        <f>D14</f>
-        <v>9.7531240475464784</v>
-      </c>
-      <c r="E22" s="23">
-        <f>12*12/162</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="F22" s="23">
-        <f t="shared" ref="F22:F23" si="1">PRODUCT(C22:E22)</f>
-        <v>86.69443597819091</v>
-      </c>
-      <c r="G22" s="23">
-        <f t="shared" ref="G22:G23" si="2">F22/1000</f>
-        <v>8.6694435978190904E-2</v>
       </c>
       <c r="H22" s="29"/>
       <c r="I22" s="29"/>
       <c r="J22" s="29"/>
       <c r="K22" s="29"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="59"/>
-      <c r="B23" s="45"/>
+      <c r="B23" s="45" t="s">
+        <v>58</v>
+      </c>
       <c r="C23" s="22">
-        <f>3*5</f>
-        <v>15</v>
+        <f>2*5</f>
+        <v>10</v>
       </c>
       <c r="D23" s="30">
-        <f>E14</f>
-        <v>5.6894239561109421</v>
+        <f>D14</f>
+        <v>9.7531240475464784</v>
       </c>
       <c r="E23" s="23">
         <f>12*12/162</f>
         <v>0.88888888888888884</v>
       </c>
       <c r="F23" s="23">
-        <f t="shared" si="1"/>
-        <v>75.858986081479216</v>
+        <f t="shared" ref="F23:F24" si="1">PRODUCT(C23:E23)</f>
+        <v>86.69443597819091</v>
       </c>
       <c r="G23" s="23">
-        <f t="shared" si="2"/>
-        <v>7.5858986081479216E-2</v>
+        <f t="shared" ref="G23:G24" si="2">F23/1000</f>
+        <v>8.6694435978190904E-2</v>
       </c>
       <c r="H23" s="29"/>
       <c r="I23" s="29"/>
       <c r="J23" s="29"/>
       <c r="K23" s="29"/>
     </row>
-    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="59"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="22">
+        <f>3*5</f>
+        <v>15</v>
+      </c>
+      <c r="D24" s="30">
+        <f>E14</f>
+        <v>5.6894239561109421</v>
+      </c>
+      <c r="E24" s="23">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F24" s="23">
+        <f t="shared" si="1"/>
+        <v>75.858986081479216</v>
+      </c>
+      <c r="G24" s="23">
+        <f t="shared" si="2"/>
+        <v>7.5858986081479216E-2</v>
+      </c>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+    </row>
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C25" s="11">
         <f>37*4</f>
         <v>148</v>
-      </c>
-      <c r="D24" s="12">
-        <f>(0.3*2+(0.583/3.281)*2+0.075*2)</f>
-        <v>1.1053794574824747</v>
-      </c>
-      <c r="E24" s="13">
-        <f t="shared" ref="E24:E25" si="3">8*8/162</f>
-        <v>0.39506172839506171</v>
-      </c>
-      <c r="F24" s="20">
-        <f>PRODUCT(C24:E24)</f>
-        <v>64.630581612802473</v>
-      </c>
-      <c r="G24" s="20">
-        <f>F24/1000</f>
-        <v>6.4630581612802468E-2</v>
-      </c>
-      <c r="H24" s="15"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="13"/>
-    </row>
-    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="11">
-        <f>(29+7+7)*3</f>
-        <v>129</v>
       </c>
       <c r="D25" s="12">
         <f>(0.3*2+(0.583/3.281)*2+0.075*2)</f>
         <v>1.1053794574824747</v>
       </c>
       <c r="E25" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E25:E26" si="3">8*8/162</f>
         <v>0.39506172839506171</v>
       </c>
       <c r="F25" s="20">
         <f>PRODUCT(C25:E25)</f>
-        <v>56.333412351699451</v>
+        <v>64.630581612802473</v>
       </c>
       <c r="G25" s="20">
         <f>F25/1000</f>
-        <v>5.6333412351699454E-2</v>
+        <v>6.4630581612802468E-2</v>
       </c>
       <c r="H25" s="15"/>
       <c r="I25" s="14"/>
       <c r="J25" s="16"/>
       <c r="K25" s="13"/>
     </row>
-    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
-      <c r="B26" s="10" t="s">
-        <v>64</v>
-      </c>
+      <c r="B26" s="10"/>
       <c r="C26" s="11">
-        <v>4</v>
+        <f>(29+7+7)*3</f>
+        <v>129</v>
       </c>
       <c r="D26" s="12">
-        <f>(6.833+0.75)/3.281</f>
-        <v>2.3111856141420297</v>
+        <f>(0.3*2+(0.583/3.281)*2+0.075*2)</f>
+        <v>1.1053794574824747</v>
       </c>
       <c r="E26" s="13">
-        <f>12*12/162</f>
-        <v>0.88888888888888884</v>
+        <f t="shared" si="3"/>
+        <v>0.39506172839506171</v>
       </c>
       <c r="F26" s="20">
-        <f t="shared" ref="F26:F27" si="4">PRODUCT(C26:E26)</f>
-        <v>8.2175488502827712</v>
+        <f>PRODUCT(C26:E26)</f>
+        <v>56.333412351699451</v>
       </c>
       <c r="G26" s="20">
-        <f t="shared" ref="G26:G27" si="5">F26/1000</f>
-        <v>8.2175488502827711E-3</v>
+        <f>F26/1000</f>
+        <v>5.6333412351699454E-2</v>
       </c>
       <c r="H26" s="15"/>
       <c r="I26" s="14"/>
       <c r="J26" s="16"/>
       <c r="K26" s="13"/>
     </row>
-    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
-      <c r="B27" s="10"/>
+      <c r="B27" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="C27" s="11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D27" s="12">
-        <f>10.75/3.281</f>
-        <v>3.2764401097226452</v>
+        <f>(6.833+0.75)/3.281</f>
+        <v>2.3111856141420297</v>
       </c>
       <c r="E27" s="13">
         <f>12*12/162</f>
         <v>0.88888888888888884</v>
       </c>
       <c r="F27" s="20">
-        <f t="shared" si="4"/>
-        <v>5.8247824172847027</v>
+        <f t="shared" ref="F27:F28" si="4">PRODUCT(C27:E27)</f>
+        <v>8.2175488502827712</v>
       </c>
       <c r="G27" s="20">
-        <f t="shared" si="5"/>
-        <v>5.824782417284703E-3</v>
+        <f t="shared" ref="G27:G28" si="5">F27/1000</f>
+        <v>8.2175488502827711E-3</v>
       </c>
       <c r="H27" s="15"/>
       <c r="I27" s="14"/>
       <c r="J27" s="16"/>
       <c r="K27" s="13"/>
     </row>
-    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="10"/>
       <c r="C28" s="11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D28" s="12">
-        <f>(4.5+2.5+0.75)/3.281</f>
-        <v>2.3620847302651629</v>
+        <f>10.75/3.281</f>
+        <v>3.2764401097226452</v>
       </c>
       <c r="E28" s="13">
         <f>12*12/162</f>
         <v>0.88888888888888884</v>
       </c>
       <c r="F28" s="20">
-        <f>PRODUCT(C28:E28)</f>
-        <v>12.597785228080866</v>
+        <f t="shared" si="4"/>
+        <v>5.8247824172847027</v>
       </c>
       <c r="G28" s="20">
-        <f>F28/1000</f>
-        <v>1.2597785228080867E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.824782417284703E-3</v>
       </c>
       <c r="H28" s="15"/>
       <c r="I28" s="14"/>
       <c r="J28" s="16"/>
       <c r="K28" s="13"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="59"/>
-      <c r="B29" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="22">
-        <f>2*5</f>
-        <v>10</v>
-      </c>
-      <c r="D29" s="30">
-        <f>(13.75-0.333+2*(7/12/3.281))</f>
-        <v>13.772582647566798</v>
+    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="11">
+        <v>6</v>
+      </c>
+      <c r="D29" s="12">
+        <f>(4.5+2.5+0.75)/3.281</f>
+        <v>2.3620847302651629</v>
       </c>
       <c r="E29" s="13">
         <f>12*12/162</f>
@@ -1982,115 +1981,117 @@
       </c>
       <c r="F29" s="20">
         <f>PRODUCT(C29:E29)</f>
-        <v>122.42295686726042</v>
+        <v>12.597785228080866</v>
       </c>
       <c r="G29" s="20">
         <f>F29/1000</f>
+        <v>1.2597785228080867E-2</v>
+      </c>
+      <c r="H29" s="15"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="13"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="59"/>
+      <c r="B30" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="22">
+        <f>2*5</f>
+        <v>10</v>
+      </c>
+      <c r="D30" s="30">
+        <f>(13.75-0.333+2*(7/12/3.281))</f>
+        <v>13.772582647566798</v>
+      </c>
+      <c r="E30" s="13">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F30" s="20">
+        <f>PRODUCT(C30:E30)</f>
+        <v>122.42295686726042</v>
+      </c>
+      <c r="G30" s="20">
+        <f>F30/1000</f>
         <v>0.12242295686726043</v>
       </c>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-    </row>
-    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="10" t="s">
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+    </row>
+    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C31" s="11">
         <f>(29)*2</f>
         <v>58</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D31" s="12">
         <f>(0.3*2+(0.583/3.281)*2+0.075*2)</f>
         <v>1.1053794574824747</v>
       </c>
-      <c r="E30" s="13">
-        <f t="shared" ref="E30" si="6">8*8/162</f>
+      <c r="E31" s="13">
+        <f t="shared" ref="E31" si="6">8*8/162</f>
         <v>0.39506172839506171</v>
       </c>
-      <c r="F30" s="20">
-        <f>PRODUCT(C30:E30)</f>
+      <c r="F31" s="20">
+        <f>PRODUCT(C31:E31)</f>
         <v>25.328200902314478</v>
       </c>
-      <c r="G30" s="20">
-        <f>F30/1000</f>
+      <c r="G31" s="20">
+        <f>F31/1000</f>
         <v>2.5328200902314479E-2</v>
-      </c>
-      <c r="H30" s="15"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="13"/>
-    </row>
-    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="11">
-        <v>4</v>
-      </c>
-      <c r="D31" s="12">
-        <f>0.3*(13.75-0.75)/3.281</f>
-        <v>1.1886619932947271</v>
-      </c>
-      <c r="E31" s="13">
-        <f>12*12/162</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="F31" s="20">
-        <f t="shared" ref="F31" si="7">PRODUCT(C31:E31)</f>
-        <v>4.2263537539368077</v>
-      </c>
-      <c r="G31" s="88">
-        <f t="shared" ref="G31" si="8">F31/1000</f>
-        <v>4.2263537539368075E-3</v>
       </c>
       <c r="H31" s="15"/>
       <c r="I31" s="14"/>
       <c r="J31" s="16"/>
       <c r="K31" s="13"/>
     </row>
-    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C32" s="11">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="D32" s="12">
-        <f>31.667/3.281</f>
-        <v>9.6516306004266994</v>
+        <f>0.3*(13.75-0.75)/3.281</f>
+        <v>1.1886619932947271</v>
       </c>
       <c r="E32" s="13">
-        <f>8*8/162</f>
-        <v>0.39506172839506171</v>
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
       </c>
       <c r="F32" s="20">
-        <f>PRODUCT(C32:E32)</f>
-        <v>129.64165547239813</v>
-      </c>
-      <c r="G32" s="20">
-        <f>F32/1000</f>
-        <v>0.12964165547239812</v>
+        <f t="shared" ref="F32" si="7">PRODUCT(C32:E32)</f>
+        <v>4.2263537539368077</v>
+      </c>
+      <c r="G32" s="66">
+        <f t="shared" ref="G32" si="8">F32/1000</f>
+        <v>4.2263537539368075E-3</v>
       </c>
       <c r="H32" s="15"/>
       <c r="I32" s="14"/>
       <c r="J32" s="16"/>
       <c r="K32" s="13"/>
     </row>
-    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
-      <c r="B33" s="10"/>
+      <c r="B33" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="C33" s="11">
-        <f>60</f>
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D33" s="12">
-        <f>18.42/3.281</f>
-        <v>5.6141420298689431</v>
+        <f>31.667/3.281</f>
+        <v>9.6516306004266994</v>
       </c>
       <c r="E33" s="13">
         <f>8*8/162</f>
@@ -2098,28 +2099,27 @@
       </c>
       <c r="F33" s="20">
         <f>PRODUCT(C33:E33)</f>
-        <v>133.07595922652308</v>
+        <v>129.64165547239813</v>
       </c>
       <c r="G33" s="20">
         <f>F33/1000</f>
-        <v>0.13307595922652307</v>
+        <v>0.12964165547239812</v>
       </c>
       <c r="H33" s="15"/>
       <c r="I33" s="14"/>
       <c r="J33" s="16"/>
       <c r="K33" s="13"/>
     </row>
-    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
-      <c r="B34" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="B34" s="10"/>
       <c r="C34" s="11">
-        <f>2*(6*2+1)</f>
-        <v>26</v>
+        <f>60</f>
+        <v>60</v>
       </c>
       <c r="D34" s="12">
-        <v>1.8</v>
+        <f>18.42/3.281</f>
+        <v>5.6141420298689431</v>
       </c>
       <c r="E34" s="13">
         <f>8*8/162</f>
@@ -2127,85 +2127,86 @@
       </c>
       <c r="F34" s="20">
         <f>PRODUCT(C34:E34)</f>
-        <v>18.488888888888891</v>
+        <v>133.07595922652308</v>
       </c>
       <c r="G34" s="20">
         <f>F34/1000</f>
-        <v>1.8488888888888892E-2</v>
+        <v>0.13307595922652307</v>
       </c>
       <c r="H34" s="15"/>
       <c r="I34" s="14"/>
       <c r="J34" s="16"/>
       <c r="K34" s="13"/>
     </row>
-    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C35" s="11">
-        <f>10*2</f>
-        <v>20</v>
+        <f>2*(6*2+1)</f>
+        <v>26</v>
       </c>
       <c r="D35" s="12">
-        <f>6.5/3.281</f>
-        <v>1.9811033221578787</v>
+        <v>1.8</v>
       </c>
       <c r="E35" s="13">
-        <f t="shared" ref="E35:E40" si="9">8*8/162</f>
+        <f>8*8/162</f>
         <v>0.39506172839506171</v>
       </c>
       <c r="F35" s="20">
-        <f t="shared" ref="F35:F40" si="10">PRODUCT(C35:E35)</f>
-        <v>15.653162051617805</v>
+        <f>PRODUCT(C35:E35)</f>
+        <v>18.488888888888891</v>
       </c>
       <c r="G35" s="20">
-        <f t="shared" ref="G35:G40" si="11">F35/1000</f>
-        <v>1.5653162051617805E-2</v>
+        <f>F35/1000</f>
+        <v>1.8488888888888892E-2</v>
       </c>
       <c r="H35" s="15"/>
       <c r="I35" s="14"/>
       <c r="J35" s="16"/>
       <c r="K35" s="13"/>
     </row>
-    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
-      <c r="B36" s="10"/>
+      <c r="B36" s="10" t="s">
+        <v>67</v>
+      </c>
       <c r="C36" s="11">
-        <f>8</f>
-        <v>8</v>
+        <f>10*2</f>
+        <v>20</v>
       </c>
       <c r="D36" s="12">
-        <f>7.5/3.281</f>
-        <v>2.2858884486437061</v>
+        <f>6.5/3.281</f>
+        <v>1.9811033221578787</v>
       </c>
       <c r="E36" s="13">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="E36:E41" si="9">8*8/162</f>
         <v>0.39506172839506171</v>
       </c>
       <c r="F36" s="20">
-        <f t="shared" si="10"/>
-        <v>7.2245363315159103</v>
+        <f t="shared" ref="F36:F41" si="10">PRODUCT(C36:E36)</f>
+        <v>15.653162051617805</v>
       </c>
       <c r="G36" s="20">
-        <f t="shared" si="11"/>
-        <v>7.2245363315159104E-3</v>
+        <f t="shared" ref="G36:G41" si="11">F36/1000</f>
+        <v>1.5653162051617805E-2</v>
       </c>
       <c r="H36" s="15"/>
       <c r="I36" s="14"/>
       <c r="J36" s="16"/>
       <c r="K36" s="13"/>
     </row>
-    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="10"/>
       <c r="C37" s="11">
-        <f>12+12</f>
-        <v>24</v>
+        <f>8</f>
+        <v>8</v>
       </c>
       <c r="D37" s="12">
-        <f>31.667/3.281</f>
-        <v>9.6516306004266994</v>
+        <f>7.5/3.281</f>
+        <v>2.2858884486437061</v>
       </c>
       <c r="E37" s="13">
         <f t="shared" si="9"/>
@@ -2213,29 +2214,27 @@
       </c>
       <c r="F37" s="20">
         <f t="shared" si="10"/>
-        <v>91.511756804045731</v>
+        <v>7.2245363315159103</v>
       </c>
       <c r="G37" s="20">
         <f t="shared" si="11"/>
-        <v>9.1511756804045732E-2</v>
+        <v>7.2245363315159104E-3</v>
       </c>
       <c r="H37" s="15"/>
       <c r="I37" s="14"/>
       <c r="J37" s="16"/>
       <c r="K37" s="13"/>
     </row>
-    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
-      <c r="B38" s="10" t="s">
-        <v>68</v>
-      </c>
+      <c r="B38" s="10"/>
       <c r="C38" s="11">
-        <f>10*2</f>
-        <v>20</v>
+        <f>12+12</f>
+        <v>24</v>
       </c>
       <c r="D38" s="12">
-        <f>7.083/3.281</f>
-        <v>2.1587930508991162</v>
+        <f>31.667/3.281</f>
+        <v>9.6516306004266994</v>
       </c>
       <c r="E38" s="13">
         <f t="shared" si="9"/>
@@ -2243,422 +2242,438 @@
       </c>
       <c r="F38" s="20">
         <f t="shared" si="10"/>
-        <v>17.057130278709067</v>
+        <v>91.511756804045731</v>
       </c>
       <c r="G38" s="20">
         <f t="shared" si="11"/>
-        <v>1.7057130278709066E-2</v>
+        <v>9.1511756804045732E-2</v>
       </c>
       <c r="H38" s="15"/>
       <c r="I38" s="14"/>
       <c r="J38" s="16"/>
       <c r="K38" s="13"/>
     </row>
-    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
-      <c r="B39" s="10"/>
+      <c r="B39" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="C39" s="11">
-        <f>12*2</f>
-        <v>24</v>
+        <f>10*2</f>
+        <v>20</v>
       </c>
       <c r="D39" s="12">
-        <f>6.583/3.281</f>
-        <v>2.0064004876562023</v>
+        <f>7.083/3.281</f>
+        <v>2.1587930508991162</v>
       </c>
       <c r="E39" s="13">
         <f t="shared" si="9"/>
         <v>0.39506172839506171</v>
       </c>
       <c r="F39" s="20">
-        <f t="shared" ref="F39" si="12">PRODUCT(C39:E39)</f>
-        <v>19.023649068147694</v>
+        <f t="shared" si="10"/>
+        <v>17.057130278709067</v>
       </c>
       <c r="G39" s="20">
-        <f t="shared" ref="G39" si="13">F39/1000</f>
-        <v>1.9023649068147696E-2</v>
+        <f t="shared" si="11"/>
+        <v>1.7057130278709066E-2</v>
       </c>
       <c r="H39" s="15"/>
       <c r="I39" s="14"/>
       <c r="J39" s="16"/>
       <c r="K39" s="13"/>
     </row>
-    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="10"/>
       <c r="C40" s="11">
-        <f>39</f>
-        <v>39</v>
+        <f>12*2</f>
+        <v>24</v>
       </c>
       <c r="D40" s="12">
-        <f>18.42/3.281</f>
-        <v>5.6141420298689431</v>
+        <f>6.583/3.281</f>
+        <v>2.0064004876562023</v>
       </c>
       <c r="E40" s="13">
         <f t="shared" si="9"/>
         <v>0.39506172839506171</v>
       </c>
       <c r="F40" s="20">
-        <f t="shared" si="10"/>
-        <v>86.499373497240001</v>
+        <f t="shared" ref="F40" si="12">PRODUCT(C40:E40)</f>
+        <v>19.023649068147694</v>
       </c>
       <c r="G40" s="20">
-        <f t="shared" si="11"/>
-        <v>8.6499373497240004E-2</v>
+        <f t="shared" ref="G40" si="13">F40/1000</f>
+        <v>1.9023649068147696E-2</v>
       </c>
       <c r="H40" s="15"/>
       <c r="I40" s="14"/>
       <c r="J40" s="16"/>
       <c r="K40" s="13"/>
     </row>
-    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
-      <c r="B41" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="14">
-        <f>SUM(G20:G40)</f>
-        <v>1.037623498707485</v>
-      </c>
-      <c r="H41" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="I41" s="14">
-        <v>131940</v>
-      </c>
-      <c r="J41" s="16">
-        <f>G41*I41</f>
-        <v>136904.04441946559</v>
-      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="11">
+        <f>39</f>
+        <v>39</v>
+      </c>
+      <c r="D41" s="12">
+        <f>18.42/3.281</f>
+        <v>5.6141420298689431</v>
+      </c>
+      <c r="E41" s="13">
+        <f t="shared" si="9"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F41" s="20">
+        <f t="shared" si="10"/>
+        <v>86.499373497240001</v>
+      </c>
+      <c r="G41" s="20">
+        <f t="shared" si="11"/>
+        <v>8.6499373497240004E-2</v>
+      </c>
+      <c r="H41" s="15"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="16"/>
       <c r="K41" s="13"/>
     </row>
-    <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="12"/>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="14"/>
+      <c r="G42" s="14">
+        <f>SUM(G21:G41)</f>
+        <v>1.037623498707485</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I42" s="14">
+        <v>131940</v>
+      </c>
       <c r="J42" s="16">
-        <f>0.13*G41*106200</f>
+        <f>G42*I42</f>
+        <v>136904.04441946559</v>
+      </c>
+      <c r="K42" s="13"/>
+    </row>
+    <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="9"/>
+      <c r="B43" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="11"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="16">
+        <f>0.13*G42*106200</f>
         <v>14325.430023155539</v>
       </c>
-      <c r="K42" s="13"/>
-    </row>
-    <row r="43" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="59"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
-    </row>
-    <row r="44" spans="1:11" s="8" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="59">
+      <c r="K43" s="13"/>
+    </row>
+    <row r="44" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="59"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+    </row>
+    <row r="45" spans="1:11" s="8" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="59">
         <v>3</v>
       </c>
-      <c r="B44" s="84" t="s">
+      <c r="B45" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
-      <c r="K44" s="44"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="59"/>
-      <c r="B45" s="45" t="str">
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="44"/>
+      <c r="H45" s="44"/>
+      <c r="I45" s="44"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="44"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="59"/>
+      <c r="B46" s="45" t="str">
         <f>B10</f>
         <v>-Column</v>
       </c>
-      <c r="C45" s="87">
+      <c r="C46" s="65">
         <f>C10</f>
         <v>6</v>
       </c>
-      <c r="D45" s="86">
+      <c r="D46" s="64">
         <v>0.3</v>
       </c>
-      <c r="E45" s="86">
+      <c r="E46" s="64">
         <v>0.3</v>
       </c>
-      <c r="F45" s="86">
+      <c r="F46" s="64">
         <f>F10</f>
         <v>2.48796098750381</v>
       </c>
-      <c r="G45" s="30">
-        <f>PRODUCT(C45:F45)</f>
+      <c r="G46" s="30">
+        <f>PRODUCT(C46:F46)</f>
         <v>1.3434989332520573</v>
-      </c>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="59"/>
-      <c r="B46" s="45" t="str">
-        <f>B11</f>
-        <v>-Beam</v>
-      </c>
-      <c r="C46" s="87">
-        <f>C11</f>
-        <v>4</v>
-      </c>
-      <c r="D46" s="86">
-        <f>D11</f>
-        <v>3.6574215178299299</v>
-      </c>
-      <c r="E46" s="86">
-        <v>0.23</v>
-      </c>
-      <c r="F46" s="86">
-        <v>0.23</v>
-      </c>
-      <c r="G46" s="30">
-        <f t="shared" ref="G46:G49" si="14">PRODUCT(C46:F46)</f>
-        <v>0.77391039317281318</v>
       </c>
       <c r="H46" s="29"/>
       <c r="I46" s="29"/>
       <c r="J46" s="29"/>
       <c r="K46" s="29"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="59"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="87">
-        <f>C12</f>
-        <v>3</v>
-      </c>
-      <c r="D47" s="86">
-        <f>D12</f>
-        <v>3.5812252362084727</v>
-      </c>
-      <c r="E47" s="86">
+      <c r="B47" s="45" t="str">
+        <f>B11</f>
+        <v>-Beam</v>
+      </c>
+      <c r="C47" s="65">
+        <f>C11</f>
+        <v>4</v>
+      </c>
+      <c r="D47" s="64">
+        <f>D11</f>
+        <v>3.6574215178299299</v>
+      </c>
+      <c r="E47" s="64">
         <v>0.23</v>
       </c>
-      <c r="F47" s="86">
+      <c r="F47" s="64">
         <v>0.23</v>
       </c>
       <c r="G47" s="30">
-        <f t="shared" si="14"/>
-        <v>0.56834044498628455</v>
+        <f t="shared" ref="G47:G50" si="14">PRODUCT(C47:F47)</f>
+        <v>0.77391039317281318</v>
       </c>
       <c r="H47" s="29"/>
       <c r="I47" s="29"/>
       <c r="J47" s="29"/>
       <c r="K47" s="29"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="59"/>
-      <c r="B48" s="45" t="str">
-        <f>B13</f>
-        <v>-Cantilever beam</v>
-      </c>
-      <c r="C48" s="87">
-        <f>C13</f>
-        <v>10</v>
-      </c>
-      <c r="D48" s="86">
-        <f>D13</f>
-        <v>0.76196281621456874</v>
-      </c>
-      <c r="E48" s="86">
+      <c r="B48" s="45"/>
+      <c r="C48" s="65">
+        <f>C12</f>
+        <v>3</v>
+      </c>
+      <c r="D48" s="64">
+        <f>D12</f>
+        <v>3.5812252362084727</v>
+      </c>
+      <c r="E48" s="64">
         <v>0.23</v>
       </c>
-      <c r="F48" s="86">
+      <c r="F48" s="64">
         <v>0.23</v>
       </c>
       <c r="G48" s="30">
         <f t="shared" si="14"/>
-        <v>0.40307832977750691</v>
+        <v>0.56834044498628455</v>
       </c>
       <c r="H48" s="29"/>
       <c r="I48" s="29"/>
       <c r="J48" s="29"/>
       <c r="K48" s="29"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="59"/>
       <c r="B49" s="45" t="str">
-        <f>B14</f>
-        <v>-Slab</v>
-      </c>
-      <c r="C49" s="87">
-        <f>C14</f>
-        <v>1</v>
-      </c>
-      <c r="D49" s="86">
-        <f>D14</f>
-        <v>9.7531240475464784</v>
-      </c>
-      <c r="E49" s="86">
-        <f>E14</f>
-        <v>5.6894239561109421</v>
-      </c>
-      <c r="F49" s="86">
-        <v>0.125</v>
+        <f>B13</f>
+        <v>-Cantilever beam</v>
+      </c>
+      <c r="C49" s="65">
+        <f>C13</f>
+        <v>10</v>
+      </c>
+      <c r="D49" s="64">
+        <f>D13</f>
+        <v>0.76196281621456874</v>
+      </c>
+      <c r="E49" s="64">
+        <v>0.23</v>
+      </c>
+      <c r="F49" s="64">
+        <v>0.23</v>
       </c>
       <c r="G49" s="30">
         <f t="shared" si="14"/>
-        <v>6.9362072003790809</v>
+        <v>0.40307832977750691</v>
       </c>
       <c r="H49" s="29"/>
       <c r="I49" s="29"/>
       <c r="J49" s="29"/>
       <c r="K49" s="29"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="59"/>
       <c r="B50" s="45" t="str">
-        <f>B15</f>
-        <v>-deduction for hollow portion</v>
-      </c>
-      <c r="C50" s="87">
-        <f>C15</f>
-        <v>-1</v>
-      </c>
-      <c r="D50" s="86">
-        <f>D15</f>
-        <v>1.8</v>
-      </c>
-      <c r="E50" s="86">
-        <f>E15</f>
-        <v>1.8</v>
-      </c>
-      <c r="F50" s="86">
+        <f>B14</f>
+        <v>-Slab</v>
+      </c>
+      <c r="C50" s="65">
+        <f>C14</f>
+        <v>1</v>
+      </c>
+      <c r="D50" s="64">
+        <f>D14</f>
+        <v>9.7531240475464784</v>
+      </c>
+      <c r="E50" s="64">
+        <f>E14</f>
+        <v>5.6894239561109421</v>
+      </c>
+      <c r="F50" s="64">
         <v>0.125</v>
       </c>
       <c r="G50" s="30">
-        <f>PRODUCT(C50:F50)</f>
-        <v>-0.40500000000000003</v>
+        <f t="shared" si="14"/>
+        <v>6.9362072003790809</v>
       </c>
       <c r="H50" s="29"/>
       <c r="I50" s="29"/>
       <c r="J50" s="29"/>
       <c r="K50" s="29"/>
     </row>
-    <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="9"/>
-      <c r="B51" s="10" t="s">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="59"/>
+      <c r="B51" s="45" t="str">
+        <f>B15</f>
+        <v>-deduction for hollow portion</v>
+      </c>
+      <c r="C51" s="65">
+        <f>C15</f>
+        <v>-1</v>
+      </c>
+      <c r="D51" s="64">
+        <f>D15</f>
+        <v>1.8</v>
+      </c>
+      <c r="E51" s="64">
+        <f>E15</f>
+        <v>1.8</v>
+      </c>
+      <c r="F51" s="64">
+        <v>0.125</v>
+      </c>
+      <c r="G51" s="30">
+        <f>PRODUCT(C51:F51)</f>
+        <v>-0.40500000000000003</v>
+      </c>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="29"/>
+      <c r="K51" s="29"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="59"/>
+      <c r="B52" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="65">
+        <v>2</v>
+      </c>
+      <c r="D52" s="64">
+        <f>12.25/3.281</f>
+        <v>3.7336177994513866</v>
+      </c>
+      <c r="E52" s="64">
+        <v>0.23</v>
+      </c>
+      <c r="F52" s="64">
+        <v>0.23</v>
+      </c>
+      <c r="G52" s="30">
+        <f t="shared" ref="G52" si="15">PRODUCT(C52:F52)</f>
+        <v>0.39501676318195678</v>
+      </c>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="29"/>
+      <c r="K52" s="29"/>
+    </row>
+    <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="9"/>
+      <c r="B53" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="11"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="14">
-        <f>SUM(G45:G50)</f>
-        <v>9.6200353015677429</v>
-      </c>
-      <c r="H51" s="15" t="s">
+      <c r="C53" s="11"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="14">
+        <f>SUM(G46:G52)</f>
+        <v>10.0150520647497</v>
+      </c>
+      <c r="H53" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I51" s="14">
+      <c r="I53" s="14">
         <v>13568.9</v>
       </c>
-      <c r="J51" s="16">
-        <f>G51*I51</f>
-        <v>130533.29700344254</v>
-      </c>
-      <c r="K51" s="13"/>
-    </row>
-    <row r="52" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="9"/>
-      <c r="B52" s="10" t="s">
+      <c r="J53" s="16">
+        <f>G53*I53</f>
+        <v>135893.23996138221</v>
+      </c>
+      <c r="K53" s="13"/>
+    </row>
+    <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="9"/>
+      <c r="B54" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C52" s="11"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="16">
-        <f>0.13*G51*9524.2</f>
-        <v>11911.008228494897</v>
-      </c>
-      <c r="K52" s="13"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A53" s="59"/>
-      <c r="B53" s="29"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="29"/>
-      <c r="I53" s="29"/>
-      <c r="J53" s="29"/>
-      <c r="K53" s="29"/>
-    </row>
-    <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="9">
-        <v>4</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C54" s="11">
-        <v>1</v>
-      </c>
+      <c r="C54" s="11"/>
       <c r="D54" s="12"/>
       <c r="E54" s="13"/>
       <c r="F54" s="13"/>
-      <c r="G54" s="32">
-        <v>1</v>
-      </c>
-      <c r="H54" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="I54" s="14">
-        <v>5000</v>
-      </c>
-      <c r="J54" s="32">
-        <f>G54*I54</f>
-        <v>5000</v>
+      <c r="G54" s="14"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="16">
+        <f>0.13*G53*9524.2</f>
+        <v>12400.096653761584</v>
       </c>
       <c r="K54" s="13"/>
     </row>
-    <row r="55" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="9"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="32"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="32"/>
-      <c r="K55" s="13"/>
-    </row>
-    <row r="56" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="59"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
+      <c r="J55" s="29"/>
+      <c r="K55" s="29"/>
+    </row>
+    <row r="56" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C56" s="11">
         <v>1</v>
@@ -2667,124 +2682,123 @@
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
       <c r="G56" s="32">
-        <f t="shared" ref="G56" si="15">PRODUCT(C56:F56)</f>
         <v>1</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I56" s="14">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="J56" s="32">
         <f>G56*I56</f>
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="K56" s="13"/>
     </row>
-    <row r="57" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
-      <c r="B57" s="31"/>
+      <c r="B57" s="7"/>
       <c r="C57" s="11"/>
       <c r="D57" s="12"/>
       <c r="E57" s="13"/>
       <c r="F57" s="13"/>
-      <c r="G57" s="14"/>
+      <c r="G57" s="32"/>
       <c r="H57" s="15"/>
       <c r="I57" s="14"/>
-      <c r="J57" s="16"/>
+      <c r="J57" s="32"/>
       <c r="K57" s="13"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A58" s="21"/>
-      <c r="B58" s="42" t="s">
+    <row r="58" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="9">
+        <v>5</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" s="11">
+        <v>1</v>
+      </c>
+      <c r="D58" s="12"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="32">
+        <f t="shared" ref="G58" si="16">PRODUCT(C58:F58)</f>
+        <v>1</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I58" s="14">
+        <v>500</v>
+      </c>
+      <c r="J58" s="32">
+        <f>G58*I58</f>
+        <v>500</v>
+      </c>
+      <c r="K58" s="13"/>
+    </row>
+    <row r="59" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="9"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="13"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="21"/>
+      <c r="B60" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="C58" s="43"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="16">
-        <f>SUM(J10:J56)</f>
-        <v>299173.77967455855</v>
-      </c>
-      <c r="K58" s="18"/>
-    </row>
-    <row r="60" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="33"/>
-      <c r="B60" s="28" t="s">
+      <c r="C60" s="43"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="16"/>
+      <c r="I60" s="16"/>
+      <c r="J60" s="16">
+        <f>SUM(J10:J58)</f>
+        <v>391693.19700096396</v>
+      </c>
+      <c r="K60" s="18"/>
+    </row>
+    <row r="62" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="33"/>
+      <c r="B62" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C60" s="68">
-        <f>J58</f>
-        <v>299173.77967455855</v>
-      </c>
-      <c r="D60" s="68"/>
-      <c r="E60" s="20">
+      <c r="C62" s="67">
+        <f>J60</f>
+        <v>391693.19700096396</v>
+      </c>
+      <c r="D62" s="67"/>
+      <c r="E62" s="20">
         <v>100</v>
       </c>
-      <c r="F60" s="34"/>
-      <c r="G60" s="35"/>
-      <c r="H60" s="34"/>
-      <c r="I60" s="36"/>
-      <c r="J60" s="37"/>
-      <c r="K60" s="38"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A61" s="39"/>
-      <c r="B61" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C61" s="71">
-        <v>250000</v>
-      </c>
-      <c r="D61" s="71"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="40"/>
-      <c r="G61" s="41"/>
-      <c r="H61" s="41"/>
-      <c r="I61" s="41"/>
-      <c r="J61" s="41"/>
-      <c r="K61" s="40"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A62" s="39"/>
-      <c r="B62" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C62" s="71">
-        <f>C61-C64-C65</f>
-        <v>237500</v>
-      </c>
-      <c r="D62" s="71"/>
-      <c r="E62" s="20">
-        <f>C62/C60*100</f>
-        <v>79.385299159021443</v>
-      </c>
-      <c r="F62" s="40"/>
-      <c r="G62" s="41"/>
-      <c r="H62" s="41"/>
-      <c r="I62" s="41"/>
-      <c r="J62" s="41"/>
-      <c r="K62" s="40"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F62" s="34"/>
+      <c r="G62" s="35"/>
+      <c r="H62" s="34"/>
+      <c r="I62" s="36"/>
+      <c r="J62" s="37"/>
+      <c r="K62" s="38"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="39"/>
       <c r="B63" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C63" s="68">
-        <f>C60-C62</f>
-        <v>61673.779674558551</v>
-      </c>
-      <c r="D63" s="68"/>
-      <c r="E63" s="20">
-        <f>100-E62</f>
-        <v>20.614700840978557</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C63" s="70">
+        <v>250000</v>
+      </c>
+      <c r="D63" s="70"/>
+      <c r="E63" s="20"/>
       <c r="F63" s="40"/>
       <c r="G63" s="41"/>
       <c r="H63" s="41"/>
@@ -2792,18 +2806,19 @@
       <c r="J63" s="41"/>
       <c r="K63" s="40"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="39"/>
       <c r="B64" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C64" s="68">
-        <f>C61*0.03</f>
-        <v>7500</v>
-      </c>
-      <c r="D64" s="68"/>
+        <v>32</v>
+      </c>
+      <c r="C64" s="70">
+        <f>C63-C66-C67</f>
+        <v>237500</v>
+      </c>
+      <c r="D64" s="70"/>
       <c r="E64" s="20">
-        <v>3</v>
+        <f>C64/C62*100</f>
+        <v>60.63419069272615</v>
       </c>
       <c r="F64" s="40"/>
       <c r="G64" s="41"/>
@@ -2812,18 +2827,19 @@
       <c r="J64" s="41"/>
       <c r="K64" s="40"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="39"/>
       <c r="B65" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C65" s="68">
-        <f>C61*0.02</f>
-        <v>5000</v>
-      </c>
-      <c r="D65" s="68"/>
+        <v>33</v>
+      </c>
+      <c r="C65" s="67">
+        <f>C62-C64</f>
+        <v>154193.19700096396</v>
+      </c>
+      <c r="D65" s="67"/>
       <c r="E65" s="20">
-        <v>2</v>
+        <f>100-E64</f>
+        <v>39.36580930727385</v>
       </c>
       <c r="F65" s="40"/>
       <c r="G65" s="41"/>
@@ -2832,16 +2848,48 @@
       <c r="J65" s="41"/>
       <c r="K65" s="40"/>
     </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="39"/>
+      <c r="B66" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C66" s="67">
+        <f>C63*0.03</f>
+        <v>7500</v>
+      </c>
+      <c r="D66" s="67"/>
+      <c r="E66" s="20">
+        <v>3</v>
+      </c>
+      <c r="F66" s="40"/>
+      <c r="G66" s="41"/>
+      <c r="H66" s="41"/>
+      <c r="I66" s="41"/>
+      <c r="J66" s="41"/>
+      <c r="K66" s="40"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="39"/>
+      <c r="B67" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C67" s="67">
+        <f>C63*0.02</f>
+        <v>5000</v>
+      </c>
+      <c r="D67" s="67"/>
+      <c r="E67" s="20">
+        <v>2</v>
+      </c>
+      <c r="F67" s="40"/>
+      <c r="G67" s="41"/>
+      <c r="H67" s="41"/>
+      <c r="I67" s="41"/>
+      <c r="J67" s="41"/>
+      <c r="K67" s="40"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -2849,9 +2897,23 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPrepared By:&amp;CChecked By:&amp;RApproved By:</oddFooter>
+  </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="57" max="16383" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
 
@@ -2863,107 +2925,107 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="13" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
-      <c r="K1" s="81"/>
-    </row>
-    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="82" t="s">
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+    </row>
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-    </row>
-    <row r="3" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="66" t="s">
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+    </row>
+    <row r="3" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-    </row>
-    <row r="4" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="66" t="s">
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+    </row>
+    <row r="4" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-    </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="83" t="s">
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="46" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="46"/>
-      <c r="C6" s="79" t="e">
+      <c r="C6" s="77" t="e">
         <f>F29</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="80"/>
+      <c r="D6" s="78"/>
       <c r="E6" s="47"/>
       <c r="F6" s="46"/>
       <c r="G6" s="46"/>
@@ -2971,90 +3033,90 @@
         <v>38</v>
       </c>
       <c r="I6" s="46"/>
-      <c r="J6" s="79" t="e">
+      <c r="J6" s="77" t="e">
         <f>I29</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="80"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="78"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
         <v>39</v>
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="48"/>
       <c r="D7" s="48"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="I7" s="76" t="s">
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="I7" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="76"/>
-      <c r="K7" s="76"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="62" t="str">
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="71" t="str">
         <f>Estimate!A6</f>
         <v>Project:- कालीमस्ट मन्दिर निर्माण</v>
       </c>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="I8" s="77" t="s">
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="I8" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="78" t="str">
+      <c r="J8" s="84"/>
+      <c r="K8" s="84"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="85" t="str">
         <f>Estimate!A7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="I9" s="77" t="s">
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="I9" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="J9" s="77"/>
-      <c r="K9" s="77"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="73" t="s">
+      <c r="J9" s="84"/>
+      <c r="K9" s="84"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="74" t="s">
+      <c r="D11" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74" t="s">
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="73" t="s">
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="K11" s="72" t="s">
+      <c r="K11" s="86" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="73"/>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="87"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="87"/>
       <c r="D12" s="49" t="s">
         <v>47</v>
       </c>
@@ -3073,33 +3135,33 @@
       <c r="I12" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="73"/>
-      <c r="K12" s="72"/>
-    </row>
-    <row r="13" spans="1:11" s="17" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="J12" s="87"/>
+      <c r="K12" s="86"/>
+    </row>
+    <row r="13" spans="1:11" s="17" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="60">
-        <f>Estimate!A44</f>
+        <f>Estimate!A45</f>
         <v>3</v>
       </c>
       <c r="B13" s="53" t="str">
-        <f>Estimate!B44</f>
+        <f>Estimate!B45</f>
         <v>d]lzgsf] k|of]u u/L ;'k/ :6«Sr/df l;d]G6 s+lqm6 ug]{ sfd -!M!=%M#_</v>
       </c>
       <c r="C13" s="50" t="str">
-        <f>Estimate!H51</f>
+        <f>Estimate!H53</f>
         <v>m3</v>
       </c>
       <c r="D13" s="50">
-        <f>Estimate!G51</f>
-        <v>9.6200353015677429</v>
+        <f>Estimate!G53</f>
+        <v>10.0150520647497</v>
       </c>
       <c r="E13" s="50">
-        <f>Estimate!I51</f>
+        <f>Estimate!I53</f>
         <v>13568.9</v>
       </c>
       <c r="F13" s="50">
         <f>D13*E13</f>
-        <v>130533.29700344254</v>
+        <v>135893.23996138221</v>
       </c>
       <c r="G13" s="50" t="e">
         <f>#REF!</f>
@@ -3119,18 +3181,18 @@
       </c>
       <c r="K13" s="52"/>
     </row>
-    <row r="14" spans="1:11" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="60"/>
       <c r="B14" s="58" t="str">
-        <f>Estimate!B52</f>
+        <f>Estimate!B54</f>
         <v>VAT calculation</v>
       </c>
       <c r="C14" s="50"/>
       <c r="D14" s="50"/>
       <c r="E14" s="50"/>
       <c r="F14" s="50">
-        <f>Estimate!J52</f>
-        <v>11911.008228494897</v>
+        <f>Estimate!J54</f>
+        <v>12400.096653761584</v>
       </c>
       <c r="G14" s="50"/>
       <c r="H14" s="50"/>
@@ -3144,7 +3206,7 @@
       </c>
       <c r="K14" s="52"/>
     </row>
-    <row r="15" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="28"/>
       <c r="C15" s="50"/>
@@ -3157,7 +3219,7 @@
       <c r="J15" s="51"/>
       <c r="K15" s="52"/>
     </row>
-    <row r="16" spans="1:11" s="17" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="17" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="60">
         <f>Estimate!A9</f>
         <v>1</v>
@@ -3167,20 +3229,20 @@
         <v>kmnfd]sf] kfOk / KnfOaf]8{af6 kmdf{ agfpg] sfd</v>
       </c>
       <c r="C16" s="50" t="str">
-        <f>Estimate!H16</f>
+        <f>Estimate!H17</f>
         <v>m2</v>
       </c>
       <c r="D16" s="50">
-        <f>Estimate!G16</f>
-        <v>0</v>
+        <f>Estimate!G17</f>
+        <v>88.774680461917129</v>
       </c>
       <c r="E16" s="50">
-        <f>Estimate!I16</f>
+        <f>Estimate!I17</f>
         <v>915.42</v>
       </c>
       <c r="F16" s="50">
         <f>D16*E16</f>
-        <v>0</v>
+        <v>81266.117988448168</v>
       </c>
       <c r="G16" s="50" t="e">
         <f>#REF!</f>
@@ -3200,18 +3262,18 @@
       </c>
       <c r="K16" s="52"/>
     </row>
-    <row r="17" spans="1:13" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="60"/>
       <c r="B17" s="58" t="str">
-        <f>Estimate!B17</f>
+        <f>Estimate!B18</f>
         <v>VAT calculation</v>
       </c>
       <c r="C17" s="50"/>
       <c r="D17" s="50"/>
       <c r="E17" s="50"/>
       <c r="F17" s="50">
-        <f>Estimate!J17</f>
-        <v>0</v>
+        <f>Estimate!J18</f>
+        <v>5404.2679547508551</v>
       </c>
       <c r="G17" s="50"/>
       <c r="H17" s="50"/>
@@ -3225,7 +3287,7 @@
       </c>
       <c r="K17" s="52"/>
     </row>
-    <row r="18" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="28"/>
       <c r="C18" s="50"/>
@@ -3238,25 +3300,25 @@
       <c r="J18" s="51"/>
       <c r="K18" s="52"/>
     </row>
-    <row r="19" spans="1:13" s="17" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" s="17" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="60">
-        <f>Estimate!A19</f>
+        <f>Estimate!A20</f>
         <v>2</v>
       </c>
       <c r="B19" s="53" t="str">
-        <f>Estimate!B19</f>
+        <f>Estimate!B20</f>
         <v>cf/=;L=;L= nflu kmnfd] 808L sf6\g], df]8\g] #) dL6/ ;Dd</v>
       </c>
       <c r="C19" s="50" t="str">
-        <f>Estimate!H41</f>
+        <f>Estimate!H42</f>
         <v>MT</v>
       </c>
       <c r="D19" s="50">
-        <f>Estimate!G41</f>
+        <f>Estimate!G42</f>
         <v>1.037623498707485</v>
       </c>
       <c r="E19" s="50">
-        <f>Estimate!I41</f>
+        <f>Estimate!I42</f>
         <v>131940</v>
       </c>
       <c r="F19" s="50">
@@ -3281,17 +3343,17 @@
       </c>
       <c r="K19" s="52"/>
     </row>
-    <row r="20" spans="1:13" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="60"/>
       <c r="B20" s="58" t="str">
-        <f>Estimate!B42</f>
+        <f>Estimate!B43</f>
         <v>VAT calculation</v>
       </c>
       <c r="C20" s="50"/>
       <c r="D20" s="50"/>
       <c r="E20" s="50"/>
       <c r="F20" s="50">
-        <f>Estimate!J42</f>
+        <f>Estimate!J43</f>
         <v>14325.430023155539</v>
       </c>
       <c r="G20" s="50"/>
@@ -3306,7 +3368,7 @@
       </c>
       <c r="K20" s="52"/>
     </row>
-    <row r="21" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="28"/>
       <c r="C21" s="50"/>
@@ -3319,7 +3381,7 @@
       <c r="J21" s="51"/>
       <c r="K21" s="52"/>
     </row>
-    <row r="22" spans="1:13" s="17" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="60" t="e">
         <f>Estimate!#REF!</f>
         <v>#REF!</v>
@@ -3362,7 +3424,7 @@
       </c>
       <c r="K22" s="52"/>
     </row>
-    <row r="23" spans="1:13" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="60"/>
       <c r="B23" s="58" t="e">
         <f>Estimate!#REF!</f>
@@ -3387,7 +3449,7 @@
       </c>
       <c r="K23" s="52"/>
     </row>
-    <row r="24" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
       <c r="B24" s="28"/>
       <c r="C24" s="50"/>
@@ -3401,25 +3463,25 @@
       <c r="K24" s="52"/>
       <c r="M24" s="61"/>
     </row>
-    <row r="25" spans="1:13" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="60">
-        <f>Estimate!A54</f>
+        <f>Estimate!A56</f>
         <v>4</v>
       </c>
       <c r="B25" s="53" t="str">
-        <f>Estimate!B54</f>
+        <f>Estimate!B56</f>
         <v>Provisional sum for lab test</v>
       </c>
       <c r="C25" s="50" t="str">
-        <f>Estimate!H54</f>
+        <f>Estimate!H56</f>
         <v>PS</v>
       </c>
       <c r="D25" s="50">
-        <f>Estimate!G54</f>
+        <f>Estimate!G56</f>
         <v>1</v>
       </c>
       <c r="E25" s="50">
-        <f>Estimate!I54</f>
+        <f>Estimate!I56</f>
         <v>5000</v>
       </c>
       <c r="F25" s="50">
@@ -3444,7 +3506,7 @@
       </c>
       <c r="K25" s="52"/>
     </row>
-    <row r="26" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
       <c r="B26" s="28"/>
       <c r="C26" s="50"/>
@@ -3457,25 +3519,25 @@
       <c r="J26" s="51"/>
       <c r="K26" s="52"/>
     </row>
-    <row r="27" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="60">
-        <f>Estimate!A56</f>
+        <f>Estimate!A58</f>
         <v>5</v>
       </c>
       <c r="B27" s="54" t="str">
-        <f>Estimate!B56</f>
+        <f>Estimate!B58</f>
         <v>Information board (सुचना पाटि)</v>
       </c>
       <c r="C27" s="50" t="str">
-        <f>Estimate!H56</f>
+        <f>Estimate!H58</f>
         <v>no.</v>
       </c>
       <c r="D27" s="50">
-        <f>Estimate!G56</f>
+        <f>Estimate!G58</f>
         <v>1</v>
       </c>
       <c r="E27" s="50">
-        <f>Estimate!I56</f>
+        <f>Estimate!I58</f>
         <v>500</v>
       </c>
       <c r="F27" s="50">
@@ -3500,7 +3562,7 @@
       </c>
       <c r="K27" s="52"/>
     </row>
-    <row r="28" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="28"/>
       <c r="B28" s="28"/>
       <c r="C28" s="50"/>
@@ -3513,7 +3575,7 @@
       <c r="J28" s="51"/>
       <c r="K28" s="52"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="29"/>
       <c r="B29" s="55" t="s">
         <v>48</v>
@@ -3539,6 +3601,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="I9:K9"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -3546,19 +3621,6 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:J12"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>